<commit_message>
conflicts and diagnoses plots
</commit_message>
<xml_diff>
--- a/results/Karol/results_article/4o_mini/MINIMAL_CONFLICTS.xlsx
+++ b/results/Karol/results_article/4o_mini/MINIMAL_CONFLICTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakto\Desktop\Pulpit\FaultDiagnosis\FaultDiagnosis\results_article\4o_mini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ania\LLM_and_diagnosisv2\results\Karol\results_article\4o_mini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F1C44-1DCE-4492-B919-02412C5D3B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4988D04-BF67-4ED9-BAFC-47F49AAC73D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="802" xr2:uid="{D7477BF9-CFC4-44C8-A16A-B837FBE23178}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="802" xr2:uid="{D7477BF9-CFC4-44C8-A16A-B837FBE23178}"/>
   </bookViews>
   <sheets>
     <sheet name="MINIMAL CONFLICTS" sheetId="4" r:id="rId1"/>
@@ -528,9 +528,6 @@
   </si>
   <si>
     <t>Example name</t>
-  </si>
-  <si>
-    <t>Example contant</t>
   </si>
   <si>
     <t>Observations</t>
@@ -1968,6 +1965,9 @@
 d = 1
 e = 2</t>
   </si>
+  <si>
+    <t>Example content</t>
+  </si>
 </sst>
 </file>
 
@@ -3089,22 +3089,10 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3113,7 +3101,19 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3495,172 +3495,172 @@
   <sheetPr codeName="Arkusz4"/>
   <dimension ref="B1:BP103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="S97" sqref="S97"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="258.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.6640625" defaultRowHeight="258.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="112.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="112.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="34.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="54.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="54.42578125" style="1" customWidth="1"/>
-    <col min="44" max="44" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="54.44140625" style="1" customWidth="1"/>
+    <col min="44" max="44" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="54.42578125" style="1" customWidth="1"/>
-    <col min="50" max="50" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="54.44140625" style="1" customWidth="1"/>
+    <col min="50" max="50" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="54.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="16384" width="17.7109375" style="1"/>
+    <col min="68" max="68" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="16384" width="17.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:68" ht="258.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:68" ht="258.75" customHeight="1" thickBot="1">
-      <c r="B2" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="50" t="s">
+      <c r="B2" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="50" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="50" t="s">
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="50" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="50" t="s">
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="50" t="s">
+      <c r="AG2" s="47"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="48"/>
+      <c r="AL2" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="52"/>
-      <c r="AR2" s="50" t="s">
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="48"/>
+      <c r="AR2" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
-      <c r="AW2" s="52"/>
-      <c r="AX2" s="50" t="s">
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
+      <c r="AW2" s="48"/>
+      <c r="AX2" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AY2" s="51"/>
-      <c r="AZ2" s="51"/>
-      <c r="BA2" s="51"/>
-      <c r="BB2" s="51"/>
-      <c r="BC2" s="52"/>
-      <c r="BD2" s="50" t="s">
+      <c r="AY2" s="47"/>
+      <c r="AZ2" s="47"/>
+      <c r="BA2" s="47"/>
+      <c r="BB2" s="47"/>
+      <c r="BC2" s="48"/>
+      <c r="BD2" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="BE2" s="51"/>
-      <c r="BF2" s="51"/>
-      <c r="BG2" s="51"/>
-      <c r="BH2" s="51"/>
-      <c r="BI2" s="52"/>
-      <c r="BJ2" s="50" t="s">
+      <c r="BE2" s="47"/>
+      <c r="BF2" s="47"/>
+      <c r="BG2" s="47"/>
+      <c r="BH2" s="47"/>
+      <c r="BI2" s="48"/>
+      <c r="BJ2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="BK2" s="51"/>
-      <c r="BL2" s="51"/>
-      <c r="BM2" s="51"/>
-      <c r="BN2" s="51"/>
-      <c r="BO2" s="52"/>
+      <c r="BK2" s="47"/>
+      <c r="BL2" s="47"/>
+      <c r="BM2" s="47"/>
+      <c r="BN2" s="47"/>
+      <c r="BO2" s="48"/>
     </row>
     <row r="3" spans="2:68" ht="258.75" customHeight="1" thickBot="1">
       <c r="B3" s="16" t="s">
@@ -3670,10 +3670,10 @@
         <v>112</v>
       </c>
       <c r="D3" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="E3" s="41" t="s">
         <v>113</v>
-      </c>
-      <c r="E3" s="41" t="s">
-        <v>114</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>88</v>
@@ -3870,13 +3870,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F4" s="25">
         <v>0</v>
@@ -4064,11 +4064,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="48"/>
+        <v>114</v>
+      </c>
+      <c r="D5" s="50"/>
       <c r="E5" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F5" s="25">
         <v>2</v>
@@ -4266,11 +4266,11 @@
         <v>3</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="48"/>
+        <v>114</v>
+      </c>
+      <c r="D6" s="50"/>
       <c r="E6" s="43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F6" s="25">
         <v>2</v>
@@ -4468,11 +4468,11 @@
         <v>4</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="48"/>
+        <v>114</v>
+      </c>
+      <c r="D7" s="50"/>
       <c r="E7" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F7" s="25">
         <v>2</v>
@@ -4670,11 +4670,11 @@
         <v>5</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="46"/>
+        <v>114</v>
+      </c>
+      <c r="D8" s="51"/>
       <c r="E8" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F8" s="25">
         <v>3</v>
@@ -4872,13 +4872,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>139</v>
+        <v>115</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>138</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F9" s="25">
         <v>0</v>
@@ -5062,11 +5062,11 @@
         <v>7</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="48"/>
+        <v>115</v>
+      </c>
+      <c r="D10" s="50"/>
       <c r="E10" s="43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F10" s="25">
         <v>1</v>
@@ -5264,11 +5264,11 @@
         <v>8</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="48"/>
+        <v>115</v>
+      </c>
+      <c r="D11" s="50"/>
       <c r="E11" s="43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F11" s="25">
         <v>1</v>
@@ -5466,11 +5466,11 @@
         <v>9</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="46"/>
+        <v>115</v>
+      </c>
+      <c r="D12" s="51"/>
       <c r="E12" s="43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F12" s="25">
         <v>2</v>
@@ -5668,13 +5668,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>140</v>
+        <v>116</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>139</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F13" s="25">
         <v>0</v>
@@ -5858,11 +5858,11 @@
         <v>11</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" s="48"/>
+        <v>116</v>
+      </c>
+      <c r="D14" s="50"/>
       <c r="E14" s="43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F14" s="25">
         <v>1</v>
@@ -6060,11 +6060,11 @@
         <v>12</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" s="48"/>
+        <v>116</v>
+      </c>
+      <c r="D15" s="50"/>
       <c r="E15" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F15" s="25">
         <v>1</v>
@@ -6262,11 +6262,11 @@
         <v>13</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="46"/>
+        <v>116</v>
+      </c>
+      <c r="D16" s="51"/>
       <c r="E16" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F16" s="25">
         <v>2</v>
@@ -6464,13 +6464,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="45" t="s">
-        <v>141</v>
+        <v>117</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>140</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F17" s="25">
         <v>0</v>
@@ -6654,11 +6654,11 @@
         <v>15</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="48"/>
+        <v>117</v>
+      </c>
+      <c r="D18" s="50"/>
       <c r="E18" s="43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F18" s="25">
         <v>1</v>
@@ -6856,11 +6856,11 @@
         <v>16</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="48"/>
+        <v>117</v>
+      </c>
+      <c r="D19" s="50"/>
       <c r="E19" s="43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F19" s="25">
         <v>2</v>
@@ -7058,11 +7058,11 @@
         <v>17</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" s="46"/>
+        <v>117</v>
+      </c>
+      <c r="D20" s="51"/>
       <c r="E20" s="43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F20" s="25">
         <v>1</v>
@@ -7260,13 +7260,13 @@
         <v>18</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="45" t="s">
-        <v>142</v>
+        <v>118</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>141</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F21" s="25">
         <v>0</v>
@@ -7450,11 +7450,11 @@
         <v>19</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" s="48"/>
+        <v>118</v>
+      </c>
+      <c r="D22" s="50"/>
       <c r="E22" s="43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F22" s="25">
         <v>2</v>
@@ -7652,11 +7652,11 @@
         <v>20</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" s="48"/>
+        <v>118</v>
+      </c>
+      <c r="D23" s="50"/>
       <c r="E23" s="43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F23" s="25">
         <v>2</v>
@@ -7854,11 +7854,11 @@
         <v>21</v>
       </c>
       <c r="C24" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D24" s="46"/>
+        <v>118</v>
+      </c>
+      <c r="D24" s="51"/>
       <c r="E24" s="43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F24" s="25">
         <v>3</v>
@@ -8056,13 +8056,13 @@
         <v>22</v>
       </c>
       <c r="C25" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25" s="45" t="s">
-        <v>143</v>
+        <v>119</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>142</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F25" s="25">
         <v>0</v>
@@ -8246,11 +8246,11 @@
         <v>23</v>
       </c>
       <c r="C26" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" s="48"/>
+        <v>119</v>
+      </c>
+      <c r="D26" s="50"/>
       <c r="E26" s="43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F26" s="25">
         <v>2</v>
@@ -8448,11 +8448,11 @@
         <v>24</v>
       </c>
       <c r="C27" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="48"/>
+        <v>119</v>
+      </c>
+      <c r="D27" s="50"/>
       <c r="E27" s="43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F27" s="25">
         <v>2</v>
@@ -8650,11 +8650,11 @@
         <v>25</v>
       </c>
       <c r="C28" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="46"/>
+        <v>119</v>
+      </c>
+      <c r="D28" s="51"/>
       <c r="E28" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F28" s="25">
         <v>2</v>
@@ -8852,13 +8852,13 @@
         <v>26</v>
       </c>
       <c r="C29" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="45" t="s">
-        <v>144</v>
+        <v>120</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>143</v>
       </c>
       <c r="E29" s="43" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F29" s="25">
         <v>0</v>
@@ -9044,11 +9044,11 @@
         <v>27</v>
       </c>
       <c r="C30" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="48"/>
+        <v>120</v>
+      </c>
+      <c r="D30" s="50"/>
       <c r="E30" s="43" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F30" s="25">
         <v>3</v>
@@ -9246,11 +9246,11 @@
         <v>28</v>
       </c>
       <c r="C31" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="48"/>
+        <v>120</v>
+      </c>
+      <c r="D31" s="50"/>
       <c r="E31" s="43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F31" s="25">
         <v>4</v>
@@ -9448,11 +9448,11 @@
         <v>29</v>
       </c>
       <c r="C32" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" s="48"/>
+        <v>120</v>
+      </c>
+      <c r="D32" s="50"/>
       <c r="E32" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F32" s="25">
         <v>3</v>
@@ -9650,11 +9650,11 @@
         <v>30</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="48"/>
+        <v>120</v>
+      </c>
+      <c r="D33" s="50"/>
       <c r="E33" s="43" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F33" s="25">
         <v>5</v>
@@ -9852,11 +9852,11 @@
         <v>31</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" s="48"/>
+        <v>120</v>
+      </c>
+      <c r="D34" s="50"/>
       <c r="E34" s="43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F34" s="25">
         <v>5</v>
@@ -10054,11 +10054,11 @@
         <v>32</v>
       </c>
       <c r="C35" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" s="48"/>
+        <v>120</v>
+      </c>
+      <c r="D35" s="50"/>
       <c r="E35" s="43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F35" s="25">
         <v>4</v>
@@ -10256,11 +10256,11 @@
         <v>33</v>
       </c>
       <c r="C36" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D36" s="46"/>
+        <v>120</v>
+      </c>
+      <c r="D36" s="51"/>
       <c r="E36" s="43" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F36" s="25">
         <v>3</v>
@@ -10458,13 +10458,13 @@
         <v>34</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" s="45" t="s">
-        <v>145</v>
+        <v>121</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>144</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F37" s="25">
         <v>0</v>
@@ -10652,11 +10652,11 @@
         <v>35</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D38" s="48"/>
+        <v>121</v>
+      </c>
+      <c r="D38" s="50"/>
       <c r="E38" s="43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F38" s="25">
         <v>5</v>
@@ -10854,11 +10854,11 @@
         <v>36</v>
       </c>
       <c r="C39" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D39" s="48"/>
+        <v>121</v>
+      </c>
+      <c r="D39" s="50"/>
       <c r="E39" s="43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F39" s="25">
         <v>3</v>
@@ -11056,11 +11056,11 @@
         <v>37</v>
       </c>
       <c r="C40" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="48"/>
+        <v>121</v>
+      </c>
+      <c r="D40" s="50"/>
       <c r="E40" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F40" s="25">
         <v>6</v>
@@ -11258,11 +11258,11 @@
         <v>38</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" s="48"/>
+        <v>121</v>
+      </c>
+      <c r="D41" s="50"/>
       <c r="E41" s="43" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F41" s="25">
         <v>3</v>
@@ -11460,11 +11460,11 @@
         <v>39</v>
       </c>
       <c r="C42" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42" s="48"/>
+        <v>121</v>
+      </c>
+      <c r="D42" s="50"/>
       <c r="E42" s="43" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F42" s="25">
         <v>4</v>
@@ -11662,11 +11662,11 @@
         <v>40</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" s="48"/>
+        <v>121</v>
+      </c>
+      <c r="D43" s="50"/>
       <c r="E43" s="43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F43" s="25">
         <v>5</v>
@@ -11864,11 +11864,11 @@
         <v>41</v>
       </c>
       <c r="C44" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="46"/>
+        <v>121</v>
+      </c>
+      <c r="D44" s="51"/>
       <c r="E44" s="43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F44" s="25">
         <v>4</v>
@@ -12066,13 +12066,13 @@
         <v>42</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="45" t="s">
-        <v>146</v>
+        <v>122</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>145</v>
       </c>
       <c r="E45" s="43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F45" s="25">
         <v>0</v>
@@ -12268,11 +12268,11 @@
         <v>43</v>
       </c>
       <c r="C46" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="46"/>
+        <v>122</v>
+      </c>
+      <c r="D46" s="51"/>
       <c r="E46" s="43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F46" s="25">
         <v>1</v>
@@ -12470,13 +12470,13 @@
         <v>44</v>
       </c>
       <c r="C47" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="D47" s="45" t="s">
-        <v>147</v>
+        <v>123</v>
+      </c>
+      <c r="D47" s="52" t="s">
+        <v>146</v>
       </c>
       <c r="E47" s="43" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F47" s="25">
         <v>0</v>
@@ -12666,11 +12666,11 @@
         <v>45</v>
       </c>
       <c r="C48" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48" s="46"/>
+        <v>123</v>
+      </c>
+      <c r="D48" s="51"/>
       <c r="E48" s="43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F48" s="25">
         <v>1</v>
@@ -12868,13 +12868,13 @@
         <v>46</v>
       </c>
       <c r="C49" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D49" s="45" t="s">
-        <v>148</v>
+        <v>124</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>147</v>
       </c>
       <c r="E49" s="43" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F49" s="25">
         <v>0</v>
@@ -13064,11 +13064,11 @@
         <v>47</v>
       </c>
       <c r="C50" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D50" s="48"/>
+        <v>124</v>
+      </c>
+      <c r="D50" s="50"/>
       <c r="E50" s="43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F50" s="25">
         <v>2</v>
@@ -13266,11 +13266,11 @@
         <v>48</v>
       </c>
       <c r="C51" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" s="48"/>
+        <v>124</v>
+      </c>
+      <c r="D51" s="50"/>
       <c r="E51" s="43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F51" s="25">
         <v>2</v>
@@ -13468,11 +13468,11 @@
         <v>49</v>
       </c>
       <c r="C52" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D52" s="46"/>
+        <v>124</v>
+      </c>
+      <c r="D52" s="51"/>
       <c r="E52" s="43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F52" s="25">
         <v>2</v>
@@ -13670,13 +13670,13 @@
         <v>50</v>
       </c>
       <c r="C53" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="D53" s="45" t="s">
-        <v>149</v>
+        <v>125</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>148</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F53" s="25">
         <v>0</v>
@@ -13866,11 +13866,11 @@
         <v>51</v>
       </c>
       <c r="C54" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="D54" s="48"/>
+        <v>125</v>
+      </c>
+      <c r="D54" s="50"/>
       <c r="E54" s="43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F54" s="25">
         <v>1</v>
@@ -14068,11 +14068,11 @@
         <v>52</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="D55" s="48"/>
+        <v>125</v>
+      </c>
+      <c r="D55" s="50"/>
       <c r="E55" s="43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F55" s="25">
         <v>1</v>
@@ -14270,11 +14270,11 @@
         <v>53</v>
       </c>
       <c r="C56" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="D56" s="46"/>
+        <v>125</v>
+      </c>
+      <c r="D56" s="51"/>
       <c r="E56" s="43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F56" s="25">
         <v>2</v>
@@ -14472,13 +14472,13 @@
         <v>54</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="D57" s="45" t="s">
-        <v>150</v>
+        <v>126</v>
+      </c>
+      <c r="D57" s="52" t="s">
+        <v>149</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F57" s="25">
         <v>0</v>
@@ -14668,11 +14668,11 @@
         <v>55</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="D58" s="48"/>
+        <v>126</v>
+      </c>
+      <c r="D58" s="50"/>
       <c r="E58" s="43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F58" s="25">
         <v>1</v>
@@ -14870,11 +14870,11 @@
         <v>56</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" s="48"/>
+        <v>126</v>
+      </c>
+      <c r="D59" s="50"/>
       <c r="E59" s="43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F59" s="25">
         <v>1</v>
@@ -15072,11 +15072,11 @@
         <v>57</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="D60" s="46"/>
+        <v>126</v>
+      </c>
+      <c r="D60" s="51"/>
       <c r="E60" s="43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F60" s="25">
         <v>2</v>
@@ -15274,13 +15274,13 @@
         <v>58</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D61" s="45" t="s">
-        <v>151</v>
+        <v>127</v>
+      </c>
+      <c r="D61" s="52" t="s">
+        <v>150</v>
       </c>
       <c r="E61" s="43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F61" s="25">
         <v>0</v>
@@ -15472,11 +15472,11 @@
         <v>59</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D62" s="48"/>
+        <v>127</v>
+      </c>
+      <c r="D62" s="50"/>
       <c r="E62" s="43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F62" s="25">
         <v>1</v>
@@ -15674,11 +15674,11 @@
         <v>60</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D63" s="48"/>
+        <v>127</v>
+      </c>
+      <c r="D63" s="50"/>
       <c r="E63" s="43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F63" s="25">
         <v>1</v>
@@ -15876,11 +15876,11 @@
         <v>61</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D64" s="46"/>
+        <v>127</v>
+      </c>
+      <c r="D64" s="51"/>
       <c r="E64" s="43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F64" s="25">
         <v>2</v>
@@ -16078,13 +16078,13 @@
         <v>62</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="D65" s="45" t="s">
-        <v>152</v>
+        <v>128</v>
+      </c>
+      <c r="D65" s="52" t="s">
+        <v>151</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F65" s="25">
         <v>0</v>
@@ -16274,11 +16274,11 @@
         <v>63</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="D66" s="48"/>
+        <v>128</v>
+      </c>
+      <c r="D66" s="50"/>
       <c r="E66" s="43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F66" s="25">
         <v>1</v>
@@ -16476,11 +16476,11 @@
         <v>64</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="D67" s="48"/>
+        <v>128</v>
+      </c>
+      <c r="D67" s="50"/>
       <c r="E67" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F67" s="25">
         <v>2</v>
@@ -16678,11 +16678,11 @@
         <v>65</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="D68" s="46"/>
+        <v>128</v>
+      </c>
+      <c r="D68" s="51"/>
       <c r="E68" s="43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F68" s="25">
         <v>3</v>
@@ -16880,13 +16880,13 @@
         <v>66</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D69" s="45" t="s">
-        <v>153</v>
+        <v>129</v>
+      </c>
+      <c r="D69" s="52" t="s">
+        <v>152</v>
       </c>
       <c r="E69" s="43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F69" s="25">
         <v>0</v>
@@ -17082,11 +17082,11 @@
         <v>67</v>
       </c>
       <c r="C70" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D70" s="48"/>
+        <v>129</v>
+      </c>
+      <c r="D70" s="50"/>
       <c r="E70" s="43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F70" s="25">
         <v>2</v>
@@ -17284,11 +17284,11 @@
         <v>68</v>
       </c>
       <c r="C71" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D71" s="48"/>
+        <v>129</v>
+      </c>
+      <c r="D71" s="50"/>
       <c r="E71" s="43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F71" s="25">
         <v>2</v>
@@ -17486,11 +17486,11 @@
         <v>69</v>
       </c>
       <c r="C72" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D72" s="46"/>
+        <v>129</v>
+      </c>
+      <c r="D72" s="51"/>
       <c r="E72" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F72" s="25">
         <v>3</v>
@@ -17688,13 +17688,13 @@
         <v>70</v>
       </c>
       <c r="C73" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D73" s="45" t="s">
-        <v>154</v>
+        <v>130</v>
+      </c>
+      <c r="D73" s="52" t="s">
+        <v>153</v>
       </c>
       <c r="E73" s="43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F73" s="25">
         <v>0</v>
@@ -17886,11 +17886,11 @@
         <v>71</v>
       </c>
       <c r="C74" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D74" s="48"/>
+        <v>130</v>
+      </c>
+      <c r="D74" s="50"/>
       <c r="E74" s="43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F74" s="25">
         <v>3</v>
@@ -18088,11 +18088,11 @@
         <v>72</v>
       </c>
       <c r="C75" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D75" s="48"/>
+        <v>130</v>
+      </c>
+      <c r="D75" s="50"/>
       <c r="E75" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F75" s="25">
         <v>5</v>
@@ -18290,11 +18290,11 @@
         <v>73</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D76" s="48"/>
+        <v>130</v>
+      </c>
+      <c r="D76" s="50"/>
       <c r="E76" s="43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F76" s="25">
         <v>5</v>
@@ -18492,11 +18492,11 @@
         <v>74</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D77" s="48"/>
+        <v>130</v>
+      </c>
+      <c r="D77" s="50"/>
       <c r="E77" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F77" s="25">
         <v>2</v>
@@ -18694,11 +18694,11 @@
         <v>75</v>
       </c>
       <c r="C78" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D78" s="48"/>
+        <v>130</v>
+      </c>
+      <c r="D78" s="50"/>
       <c r="E78" s="43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F78" s="25">
         <v>2</v>
@@ -18896,11 +18896,11 @@
         <v>76</v>
       </c>
       <c r="C79" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D79" s="48"/>
+        <v>130</v>
+      </c>
+      <c r="D79" s="50"/>
       <c r="E79" s="43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F79" s="25">
         <v>3</v>
@@ -19098,11 +19098,11 @@
         <v>77</v>
       </c>
       <c r="C80" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D80" s="46"/>
+        <v>130</v>
+      </c>
+      <c r="D80" s="51"/>
       <c r="E80" s="43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F80" s="25">
         <v>5</v>
@@ -19300,13 +19300,13 @@
         <v>78</v>
       </c>
       <c r="C81" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D81" s="45" t="s">
-        <v>155</v>
+        <v>131</v>
+      </c>
+      <c r="D81" s="52" t="s">
+        <v>154</v>
       </c>
       <c r="E81" s="43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F81" s="25">
         <v>0</v>
@@ -19502,11 +19502,11 @@
         <v>79</v>
       </c>
       <c r="C82" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D82" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="D82" s="50"/>
       <c r="E82" s="43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F82" s="25">
         <v>1</v>
@@ -19704,11 +19704,11 @@
         <v>80</v>
       </c>
       <c r="C83" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D83" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="D83" s="50"/>
       <c r="E83" s="43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F83" s="25">
         <v>5</v>
@@ -19906,11 +19906,11 @@
         <v>81</v>
       </c>
       <c r="C84" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D84" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="D84" s="50"/>
       <c r="E84" s="43" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F84" s="25">
         <v>3</v>
@@ -20108,11 +20108,11 @@
         <v>82</v>
       </c>
       <c r="C85" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D85" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="D85" s="50"/>
       <c r="E85" s="43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F85" s="25">
         <v>5</v>
@@ -20310,11 +20310,11 @@
         <v>83</v>
       </c>
       <c r="C86" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D86" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="D86" s="50"/>
       <c r="E86" s="43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F86" s="25">
         <v>4</v>
@@ -20512,11 +20512,11 @@
         <v>84</v>
       </c>
       <c r="C87" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D87" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="D87" s="50"/>
       <c r="E87" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F87" s="25">
         <v>1</v>
@@ -20714,11 +20714,11 @@
         <v>85</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D88" s="46"/>
+        <v>131</v>
+      </c>
+      <c r="D88" s="51"/>
       <c r="E88" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F88" s="25">
         <v>5</v>
@@ -20916,13 +20916,13 @@
         <v>86</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="D89" s="45" t="s">
-        <v>156</v>
+        <v>132</v>
+      </c>
+      <c r="D89" s="52" t="s">
+        <v>155</v>
       </c>
       <c r="E89" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F89" s="25">
         <v>0</v>
@@ -21118,11 +21118,11 @@
         <v>87</v>
       </c>
       <c r="C90" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="D90" s="48"/>
+        <v>132</v>
+      </c>
+      <c r="D90" s="50"/>
       <c r="E90" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F90" s="25">
         <v>2</v>
@@ -21320,11 +21320,11 @@
         <v>88</v>
       </c>
       <c r="C91" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="D91" s="48"/>
+        <v>132</v>
+      </c>
+      <c r="D91" s="50"/>
       <c r="E91" s="43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F91" s="25">
         <v>2</v>
@@ -21522,11 +21522,11 @@
         <v>89</v>
       </c>
       <c r="C92" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="D92" s="46"/>
+        <v>132</v>
+      </c>
+      <c r="D92" s="51"/>
       <c r="E92" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F92" s="25">
         <v>3</v>
@@ -21724,13 +21724,13 @@
         <v>90</v>
       </c>
       <c r="C93" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="D93" s="45" t="s">
-        <v>157</v>
+        <v>133</v>
+      </c>
+      <c r="D93" s="52" t="s">
+        <v>156</v>
       </c>
       <c r="E93" s="43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F93" s="25">
         <v>0</v>
@@ -21926,11 +21926,11 @@
         <v>91</v>
       </c>
       <c r="C94" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="D94" s="48"/>
+        <v>133</v>
+      </c>
+      <c r="D94" s="50"/>
       <c r="E94" s="43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F94" s="25">
         <v>2</v>
@@ -22128,11 +22128,11 @@
         <v>92</v>
       </c>
       <c r="C95" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="D95" s="48"/>
+        <v>133</v>
+      </c>
+      <c r="D95" s="50"/>
       <c r="E95" s="43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F95" s="25">
         <v>1</v>
@@ -22330,11 +22330,11 @@
         <v>93</v>
       </c>
       <c r="C96" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="D96" s="46"/>
+        <v>133</v>
+      </c>
+      <c r="D96" s="51"/>
       <c r="E96" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F96" s="25">
         <v>3</v>
@@ -22532,13 +22532,13 @@
         <v>94</v>
       </c>
       <c r="C97" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="D97" s="45" t="s">
-        <v>158</v>
+        <v>134</v>
+      </c>
+      <c r="D97" s="52" t="s">
+        <v>157</v>
       </c>
       <c r="E97" s="43" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F97" s="25">
         <v>0</v>
@@ -22734,11 +22734,11 @@
         <v>95</v>
       </c>
       <c r="C98" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="D98" s="46"/>
+        <v>134</v>
+      </c>
+      <c r="D98" s="51"/>
       <c r="E98" s="43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F98" s="25">
         <v>1</v>
@@ -22936,13 +22936,13 @@
         <v>96</v>
       </c>
       <c r="C99" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="D99" s="45" t="s">
-        <v>159</v>
+        <v>135</v>
+      </c>
+      <c r="D99" s="52" t="s">
+        <v>158</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F99" s="25">
         <f t="shared" ref="F99:F102" si="2">IF(G99="", 0, LEN(G99) - LEN(SUBSTITUTE(G99, CHAR(10), "")) + 1)</f>
@@ -23139,11 +23139,11 @@
         <v>97</v>
       </c>
       <c r="C100" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="D100" s="46"/>
+        <v>135</v>
+      </c>
+      <c r="D100" s="51"/>
       <c r="E100" s="43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F100" s="25">
         <f t="shared" si="2"/>
@@ -23342,13 +23342,13 @@
         <v>98</v>
       </c>
       <c r="C101" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="D101" s="45" t="s">
-        <v>160</v>
+        <v>136</v>
+      </c>
+      <c r="D101" s="52" t="s">
+        <v>159</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F101" s="25">
         <f t="shared" si="2"/>
@@ -23543,11 +23543,11 @@
         <v>99</v>
       </c>
       <c r="C102" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="D102" s="47"/>
+        <v>136</v>
+      </c>
+      <c r="D102" s="53"/>
       <c r="E102" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F102" s="27">
         <f t="shared" si="2"/>
@@ -23752,32 +23752,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="T2:Y2"/>
-    <mergeCell ref="Z2:AE2"/>
-    <mergeCell ref="BJ2:BO2"/>
-    <mergeCell ref="AF2:AK2"/>
-    <mergeCell ref="AL2:AQ2"/>
-    <mergeCell ref="AR2:AW2"/>
-    <mergeCell ref="AX2:BC2"/>
-    <mergeCell ref="BD2:BI2"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="D29:D36"/>
-    <mergeCell ref="D37:D44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="D65:D68"/>
     <mergeCell ref="D97:D98"/>
     <mergeCell ref="D99:D100"/>
     <mergeCell ref="D101:D102"/>
@@ -23786,6 +23760,32 @@
     <mergeCell ref="D81:D88"/>
     <mergeCell ref="D89:D92"/>
     <mergeCell ref="D93:D96"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="D29:D36"/>
+    <mergeCell ref="D37:D44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="BJ2:BO2"/>
+    <mergeCell ref="AF2:AK2"/>
+    <mergeCell ref="AL2:AQ2"/>
+    <mergeCell ref="AR2:AW2"/>
+    <mergeCell ref="AX2:BC2"/>
+    <mergeCell ref="BD2:BI2"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="T2:Y2"/>
+    <mergeCell ref="Z2:AE2"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="L1:L1048576 X2 AJ2 AV2 BH2">
@@ -24178,20 +24178,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="58f62c55-904c-45ab-921a-aadd23c9ae33" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="58f62c55-904c-45ab-921a-aadd23c9ae33" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24214,6 +24214,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDD6D5E5-ECB9-438E-99E0-1D766706DDC6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB0BEC68-A8D2-41C9-8F24-363FE6B4FCA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="f146318e-9396-49ea-b06c-cd0efdf32951"/>
@@ -24228,12 +24236,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDD6D5E5-ECB9-438E-99E0-1D766706DDC6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>